<commit_message>
15102024 5:38 optimized config UI
</commit_message>
<xml_diff>
--- a/src/assets/excel/example.xlsx
+++ b/src/assets/excel/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackliu\Desktop\Programming List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackliu\Desktop\Kasta Project Management Platform\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633D740B-C8BC-460E-A719-235352342627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71FCA80-1DA0-4CA9-A043-4D38E3C5D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13065" yWindow="30" windowWidth="15660" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40380" yWindow="435" windowWidth="16530" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Programming Details" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>KASTA DEVICE</t>
   </si>
@@ -287,12 +287,6 @@
 6: SCENE Two Way PowerPoint Type</t>
   </si>
   <si>
-    <t>r1 on
-r2 OFF
-r3, r4, r5 ON
-r6, r7, r8 OFF</t>
-  </si>
-  <si>
     <t>CONTROL CONTENT:
 d1 TURN ON
 d2 TURN OFF 
@@ -310,6 +304,19 @@
   <si>
     <t>PPT_1 ON OFF
 PPT_2 OFF ON</t>
+  </si>
+  <si>
+    <t>NAME: S2400IB2</t>
+  </si>
+  <si>
+    <t>s1
+s2</t>
+  </si>
+  <si>
+    <t>r1 on
+r2 OFF
+r3, r4, r5, s1 ON
+r6, r7, r8, s2 OFF</t>
   </si>
 </sst>
 </file>
@@ -834,10 +841,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B29" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,294 +881,303 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="11" t="s">
+    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="12" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
-      <c r="B9" s="9" t="s">
-        <v>20</v>
+      <c r="B9" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="9" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="375" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="375" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+    <row r="31" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C32" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="13" t="s">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C33" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="16"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
16102024 10:41 add new action on curtain type
</commit_message>
<xml_diff>
--- a/src/assets/excel/example.xlsx
+++ b/src/assets/excel/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackliu\Desktop\Kasta Project Management Platform\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71FCA80-1DA0-4CA9-A043-4D38E3C5D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F52088-00BD-4585-A397-974BCDF70DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40380" yWindow="435" windowWidth="16530" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33090" yWindow="120" windowWidth="16530" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Programming Details" sheetId="1" r:id="rId1"/>
@@ -249,13 +249,6 @@
 4: SCENE Relay Type - MOMENTARY</t>
   </si>
   <si>
-    <t>1: DEVICE CURTAIN_1 - CLOSE
-2: DEVICE CURTAIN_2 - OPEN
-3: DEVICE CURTAIN_3 - OPEN
-4: SCENE Mixed Type
-5: GROUP DND</t>
-  </si>
-  <si>
     <t>NAME: Single Way PowerPoint Type</t>
   </si>
   <si>
@@ -306,9 +299,6 @@
 PPT_2 OFF ON</t>
   </si>
   <si>
-    <t>NAME: S2400IB2</t>
-  </si>
-  <si>
     <t>s1
 s2</t>
   </si>
@@ -317,6 +307,16 @@
 r2 OFF
 r3, r4, r5, s1 ON
 r6, r7, r8, s2 OFF</t>
+  </si>
+  <si>
+    <t>NAME: S2400IBH</t>
+  </si>
+  <si>
+    <t>1: DEVICE CURTAIN_1 - CLOSE
+2: DEVICE CURTAIN_2 - OPEN
+3: DEVICE CURTAIN_3 - WHOLE
+4: SCENE Mixed Type
+5: GROUP DND</t>
   </si>
 </sst>
 </file>
@@ -843,8 +843,8 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>22</v>
@@ -875,7 +875,7 @@
     <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>1</v>
@@ -884,10 +884,10 @@
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>33</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1081,22 +1081,22 @@
         <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>37</v>
@@ -1156,7 +1156,7 @@
         <v>18</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
         <v>50</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
16102024 11:39 add new condition of rc_index
</commit_message>
<xml_diff>
--- a/src/assets/excel/example.xlsx
+++ b/src/assets/excel/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackliu\Desktop\Kasta Project Management Platform\src\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F52088-00BD-4585-A397-974BCDF70DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDBEB27-816F-4204-96BF-77AC70F472F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33090" yWindow="120" windowWidth="16530" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33300" yWindow="120" windowWidth="16530" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Programming Details" sheetId="1" r:id="rId1"/>
@@ -243,12 +243,6 @@
 3: SCENE Fan Type</t>
   </si>
   <si>
-    <t>1: DEVICE CURTAIN_1 - CLOSE
-2: DEVICE CURTAIN_2 - OPEN
-3: SCENE Dimmer Type - TOGGLE
-4: SCENE Relay Type - MOMENTARY</t>
-  </si>
-  <si>
     <t>NAME: Single Way PowerPoint Type</t>
   </si>
   <si>
@@ -312,11 +306,17 @@
     <t>NAME: S2400IBH</t>
   </si>
   <si>
+    <t>1: DEVICE FAN1 - FAN
+2: DEVICE FAN2 - LAMP
+3: DEVICE FAN3 - WHOLE
+4: SCENE Mixed Type</t>
+  </si>
+  <si>
     <t>1: DEVICE CURTAIN_1 - CLOSE
 2: DEVICE CURTAIN_2 - OPEN
 3: DEVICE CURTAIN_3 - WHOLE
-4: SCENE Mixed Type
-5: GROUP DND</t>
+4: SCENE Dimmer Type - TOGGLE
+5: SCENE Relay Type - MOMENTARY</t>
   </si>
 </sst>
 </file>
@@ -844,7 +844,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B30" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>22</v>
@@ -875,7 +875,7 @@
     <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>1</v>
@@ -884,10 +884,10 @@
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>33</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1081,22 +1081,22 @@
         <v>31</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>37</v>
@@ -1147,7 +1147,7 @@
         <v>17</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
         <v>50</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>